<commit_message>
added user info to data files
</commit_message>
<xml_diff>
--- a/MedPortalDOCBILL.xlsx
+++ b/MedPortalDOCBILL.xlsx
@@ -1,36 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ComputerOne\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfaul\Desktop\MidTermProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB8FC7D-DC80-449F-B186-4F2F503E03A5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D216A94F-86E5-4AD4-BCF1-C691E9EA69A7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{FBD1BDB6-E3CB-4333-8150-72B02CC78468}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>social</t>
   </si>
@@ -38,9 +33,6 @@
     <t>doc office</t>
   </si>
   <si>
-    <t>appt time</t>
-  </si>
-  <si>
     <t>doc location</t>
   </si>
   <si>
@@ -54,6 +46,51 @@
   </si>
   <si>
     <t>left to pay</t>
+  </si>
+  <si>
+    <t>apt time</t>
+  </si>
+  <si>
+    <t>812-121-0912</t>
+  </si>
+  <si>
+    <t>Dr. Bailey</t>
+  </si>
+  <si>
+    <t>Watson Clinic South</t>
+  </si>
+  <si>
+    <t>503-388-1908</t>
+  </si>
+  <si>
+    <t>Dr. Miley</t>
+  </si>
+  <si>
+    <t>East Bay Clinic</t>
+  </si>
+  <si>
+    <t>810-225-7205</t>
+  </si>
+  <si>
+    <t>Dr. Hurtak</t>
+  </si>
+  <si>
+    <t>Tampa General</t>
+  </si>
+  <si>
+    <t>011-433-3770</t>
+  </si>
+  <si>
+    <t>Dr.Bailey</t>
+  </si>
+  <si>
+    <t>800-992-2131</t>
+  </si>
+  <si>
+    <t>Dr. Mallove</t>
+  </si>
+  <si>
+    <t>Southshore Reginal</t>
   </si>
 </sst>
 </file>
@@ -104,9 +141,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB384E68-46A3-4184-9CB0-1EB9A1B64116}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,19 +482,149 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>125.75</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>49.54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>100.34</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>75.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.46875</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>